<commit_message>
Solucionada parte fechas de autor
</commit_message>
<xml_diff>
--- a/insumos/Parte1_requerimiento2y3.xlsx
+++ b/insumos/Parte1_requerimiento2y3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Emprendiendo\Capacitaciones\Desafio_Latam\Ruby_On_Rails\Bootcamp\2022.04.05_biblioteca\insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4FE49B-6AA3-4320-A357-A47E8BF63758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE503C2-1B93-4AE2-908D-804D8E0D59CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{F8C6C72E-6F90-4C8D-AE57-FB3B2C310689}"/>
   </bookViews>
@@ -143,9 +143,6 @@
     <t>SERIAL</t>
   </si>
   <si>
-    <t>DATE</t>
-  </si>
-  <si>
     <t>VARCHAR NOT NULL</t>
   </si>
   <si>
@@ -243,6 +240,9 @@
   </si>
   <si>
     <t>VARCHAR(15) NOT NULL REFERENCES libro</t>
+  </si>
+  <si>
+    <t>VARCHAR(4)</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1259,7 @@
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1272,7 +1272,7 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1285,7 +1285,7 @@
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1322,8 +1322,8 @@
   </sheetPr>
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1444,28 +1444,28 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>34</v>
@@ -1475,7 +1475,7 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>32</v>
@@ -1484,21 +1484,21 @@
         <v>22</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>32</v>
@@ -1508,28 +1508,28 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>32</v>
@@ -1539,66 +1539,66 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>23</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="7"/>
       <c r="B10" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="M10" s="9"/>
     </row>
@@ -1608,10 +1608,10 @@
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -1627,10 +1627,10 @@
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -1646,10 +1646,10 @@
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -1665,10 +1665,10 @@
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>

</xml_diff>